<commit_message>
Code change, and Removed Un-used files
</commit_message>
<xml_diff>
--- a/TestData/Testdata_Signup.xlsx
+++ b/TestData/Testdata_Signup.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srava\PycharmProjects\AluTest\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chnga\PycharmProjects\AluTest\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DD9B15-5C26-44F3-B647-374BE5874FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A2C152-9EB4-4E1D-96AD-657EA5EE5744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{3DAB58C7-9B68-49E7-9367-5E7936CE9207}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3DAB58C7-9B68-49E7-9367-5E7936CE9207}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Invalid_Testcases" sheetId="1" r:id="rId1"/>
+    <sheet name="Valid_Testcases" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="47">
   <si>
     <t>${Firstname_field}</t>
   </si>
@@ -197,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +214,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,7 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -267,6 +274,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -584,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30B81AC-82A4-4731-8860-523481D63794}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1843,4 +1858,991 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F92533B-FB3F-41EA-A260-EA5CDDCECDD2}">
+  <dimension ref="A1:F48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="11">
+        <v>12346567</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="12">
+        <v>-1234567890</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="12">
+        <v>12</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="12">
+        <v>12345678901</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E44" s="12">
+        <v>1</v>
+      </c>
+      <c r="F44" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E47" s="12">
+        <v>12345</v>
+      </c>
+      <c r="F47" s="12">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="12">
+        <v>1234567894</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B16" r:id="rId1" xr:uid="{8EF48D80-B0AD-454B-AF10-13F9813DE97A}"/>
+    <hyperlink ref="B18" r:id="rId2" xr:uid="{513A4423-85E4-46E9-9E62-1733F5261F61}"/>
+    <hyperlink ref="B19" r:id="rId3" xr:uid="{3DA0E270-C7A7-4471-9B72-A38C6EAD62BA}"/>
+    <hyperlink ref="C22" r:id="rId4" xr:uid="{3C97BA07-0D80-4CFD-89AA-A9FB35792094}"/>
+    <hyperlink ref="C25" r:id="rId5" xr:uid="{09BA6EE3-A46B-459C-BD9B-8247DA9676D6}"/>
+    <hyperlink ref="C26" r:id="rId6" xr:uid="{35C2394C-CB2B-4B3F-B7E6-27AB8902391D}"/>
+    <hyperlink ref="C27" r:id="rId7" xr:uid="{86F668E9-1D6E-45E2-BE93-3A89C21E8E56}"/>
+    <hyperlink ref="C28" r:id="rId8" xr:uid="{6470D580-D793-4540-BE5B-3B8CBD78CA58}"/>
+    <hyperlink ref="C29" r:id="rId9" xr:uid="{BFF91198-DDB4-4BCD-B270-0807CDCB01F1}"/>
+    <hyperlink ref="C30" r:id="rId10" xr:uid="{EE930571-86D5-461A-9C27-C47BD721CA2D}"/>
+    <hyperlink ref="C31" r:id="rId11" xr:uid="{EBF03599-E057-4AD5-9314-25E29390FC46}"/>
+    <hyperlink ref="C2" r:id="rId12" xr:uid="{B32CF66D-A92D-4D48-AC8B-9C807E0CC83E}"/>
+    <hyperlink ref="C3:C19" r:id="rId13" display="testemail@gmail.com" xr:uid="{2B3C7A44-D4A7-4DE5-8170-5409459A82FE}"/>
+    <hyperlink ref="C33:C42" r:id="rId14" display="testemail@gmail.com" xr:uid="{94FF54A2-2F2F-41F7-824D-82911342D9DE}"/>
+    <hyperlink ref="C43" r:id="rId15" xr:uid="{2F750324-2DBC-429E-BD35-60C504794B29}"/>
+    <hyperlink ref="C44" r:id="rId16" xr:uid="{9B36CA4D-436D-4CFF-A7ED-757BE82668E9}"/>
+    <hyperlink ref="C45" r:id="rId17" xr:uid="{6C3631C3-8683-4D90-A809-E42B3B829922}"/>
+    <hyperlink ref="C46" r:id="rId18" xr:uid="{A54CEBD7-A758-41DE-A537-247335DD35D3}"/>
+    <hyperlink ref="C47" r:id="rId19" xr:uid="{8D3A5F2D-8A24-44EE-84FF-57CAB9E1C5BA}"/>
+    <hyperlink ref="C48" r:id="rId20" xr:uid="{B20EF1D2-596B-4EBA-A041-5277A565E1D4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>